<commit_message>
Kcat curation for pooled ecYali
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujum\OneDrive\Documentos\GitHub\GECKO\ecYaliGEM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1CD604-3957-4844-9208-692D35ABEC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C983CD-857F-4B40-BDE1-FA9861EF7A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
   <si>
     <t>proteins</t>
   </si>
@@ -131,154 +131,208 @@
     <t>y000009</t>
   </si>
   <si>
+    <t>YALI0E31515g</t>
+  </si>
+  <si>
+    <t>Q6C0K8</t>
+  </si>
+  <si>
+    <t>YALI0F23837g</t>
+  </si>
+  <si>
+    <t>y000251</t>
+  </si>
+  <si>
+    <t>Brenda kcat &gt; DLKcat. Adjusted with Brenda data (highest specific activity)</t>
+  </si>
+  <si>
+    <t>Q6CGV1</t>
+  </si>
+  <si>
+    <t>YALI0A15972g</t>
+  </si>
+  <si>
+    <t>y000449</t>
+  </si>
+  <si>
+    <t>Brenda kcat &gt; DLKcat. Got the highest non-mutant value in Brenda (Salmonella enterica).</t>
+  </si>
+  <si>
+    <t>Q6CAF8</t>
+  </si>
+  <si>
+    <t>YALI0D03135g</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Got the highest value in Brenda for matching substrate (Meiothermus ruber).</t>
+  </si>
+  <si>
+    <t>y000096</t>
+  </si>
+  <si>
+    <t>Q6CDD3</t>
+  </si>
+  <si>
+    <t>YALI0C01411g</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Calculated from the specific activity of N. crassa (Brenda)</t>
+  </si>
+  <si>
+    <t>Q6C791</t>
+  </si>
+  <si>
+    <t>YALI0E02728g</t>
+  </si>
+  <si>
+    <t>y000027</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Calculated from the specific activity of S. oneidensis (Brenda EC 4.2.1.117)</t>
+  </si>
+  <si>
+    <t>Q6C564</t>
+  </si>
+  <si>
+    <t>YALI0E20691g</t>
+  </si>
+  <si>
+    <t>YALI0E07271g</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Calculated from the specific activity of M. smegmatis (Brenda EC 6.4.1.1)</t>
+  </si>
+  <si>
+    <t>Q6CAV2</t>
+  </si>
+  <si>
+    <t>y000958</t>
+  </si>
+  <si>
+    <t>y000238, y000239, y000240</t>
+  </si>
+  <si>
+    <t>Q6C231</t>
+  </si>
+  <si>
+    <t>YALI0F11297g</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Calculated from the specific activity of R. norvegicus (Brenda EC 1.14.18.9)</t>
+  </si>
+  <si>
+    <t>y000354</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Calculated from the specific activity of Candida methylica (Brenda) x10.</t>
+  </si>
+  <si>
+    <t>y000233</t>
+  </si>
+  <si>
+    <t>Q6CGM4</t>
+  </si>
+  <si>
+    <t>YALI0A18062g</t>
+  </si>
+  <si>
+    <t>Q6C968</t>
+  </si>
+  <si>
+    <t>YALI0D13596g</t>
+  </si>
+  <si>
+    <t>y000219</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 5. Calculatedby multiplying highest kcat/Km * Km (Brenda EC 1.14.19.41)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 5. Calculated from the specific activity of S. cerevisae (Ec 1.2.1.11)</t>
+  </si>
+  <si>
+    <t>y000302</t>
+  </si>
+  <si>
+    <t>Q6C5V2</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 5. Calculated from the specific activity of Y. lipolytica (Ec 4.2.1.3)</t>
+  </si>
+  <si>
+    <t>YALI0E14949g</t>
+  </si>
+  <si>
+    <t>Q6C638</t>
+  </si>
+  <si>
+    <t>YALI0E12683g</t>
+  </si>
+  <si>
+    <t>y000727</t>
+  </si>
+  <si>
+    <t>Q12726</t>
+  </si>
+  <si>
+    <t>YALI0F31075g</t>
+  </si>
+  <si>
+    <t>y001838</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Got the highest value in Brenda (EC 2.3.3.14).</t>
+  </si>
+  <si>
+    <t>Transport reaction. Kcat set to 10^3 order of magnitude</t>
+  </si>
+  <si>
+    <t>F2Z694</t>
+  </si>
+  <si>
+    <t>Q6C1W2</t>
+  </si>
+  <si>
+    <t>Q6C0B0</t>
+  </si>
+  <si>
+    <t>Q6C428</t>
+  </si>
+  <si>
+    <t>Q6C7R0</t>
+  </si>
+  <si>
+    <t>Q6CCX5</t>
+  </si>
+  <si>
+    <t>Q6C3A8</t>
+  </si>
+  <si>
     <t>Q6CAH9</t>
   </si>
   <si>
-    <t>F2Z694</t>
-  </si>
-  <si>
-    <t>Q6C1W2</t>
-  </si>
-  <si>
-    <t>Q6C0B0</t>
-  </si>
-  <si>
-    <t>Q6C428</t>
-  </si>
-  <si>
-    <t>Q6C7R0</t>
-  </si>
-  <si>
     <t>Q6CG86</t>
   </si>
   <si>
-    <t>Q6CCX5</t>
-  </si>
-  <si>
     <t>Q6C8F4</t>
   </si>
   <si>
-    <t>Q6C3A8</t>
-  </si>
-  <si>
     <t>Q6CD72 + Q6C3F1</t>
   </si>
   <si>
-    <t>y001099</t>
-  </si>
-  <si>
-    <t>y001126_REV</t>
-  </si>
-  <si>
-    <t>y001171</t>
-  </si>
-  <si>
-    <t>y001194</t>
-  </si>
-  <si>
-    <t>y001277_REV</t>
-  </si>
-  <si>
-    <t>y001665</t>
-  </si>
-  <si>
-    <t>y001887</t>
-  </si>
-  <si>
-    <t>y002034</t>
-  </si>
-  <si>
-    <t>y001110</t>
-  </si>
-  <si>
-    <t>y001115</t>
-  </si>
-  <si>
-    <t>y001244</t>
-  </si>
-  <si>
-    <t>y001245</t>
-  </si>
-  <si>
-    <t>y001254_REV</t>
-  </si>
-  <si>
-    <t>Output of sensitiveTuning. Unconstrained kcat to the 10^3 order of magnitude</t>
-  </si>
-  <si>
     <t>1 + 1</t>
   </si>
   <si>
-    <t>YALI0D02629g</t>
-  </si>
-  <si>
-    <t>YALI0D08228g</t>
-  </si>
-  <si>
-    <t>YALI0F12925g</t>
-  </si>
-  <si>
-    <t>YALI0F26323g</t>
-  </si>
-  <si>
-    <t>YALI0E31515g</t>
-  </si>
-  <si>
-    <t>YALI0E30283g</t>
-  </si>
-  <si>
-    <t>YALI0D26147g</t>
-  </si>
-  <si>
-    <t>YALI0A21307g</t>
-  </si>
-  <si>
-    <t>YALI0C05753g</t>
-  </si>
-  <si>
-    <t>YALI0D20108g</t>
-  </si>
-  <si>
-    <t>YALI0F01210g</t>
-  </si>
-  <si>
-    <t>YALI0C03223g</t>
-  </si>
-  <si>
-    <t>Q6C0K8</t>
-  </si>
-  <si>
-    <t>YALI0F23837g</t>
-  </si>
-  <si>
-    <t>y000251</t>
-  </si>
-  <si>
-    <t>Brenda kcat &gt; DLKcat. Adjusted with Brenda data (highest specific activity)</t>
-  </si>
-  <si>
-    <t>Q6CGV1</t>
-  </si>
-  <si>
-    <t>YALI0A15972g</t>
-  </si>
-  <si>
-    <t>y000449</t>
-  </si>
-  <si>
-    <t>Brenda kcat &gt; DLKcat. Got the highest non-mutant value in Brenda (Salmonella enterica).</t>
-  </si>
-  <si>
-    <t>Q6CAF8</t>
-  </si>
-  <si>
-    <t>YALI0D03135g</t>
-  </si>
-  <si>
-    <t>y000669</t>
-  </si>
-  <si>
-    <t>Output of sensitivityTuning. Got the highest value in Brenda for matching substrate (Meiothermus ruber).</t>
+    <t>y000029</t>
+  </si>
+  <si>
+    <t>Q6C120</t>
+  </si>
+  <si>
+    <t>YALI0F19910g</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3.  Calculated from the specific activity of N. crassa (Brenda)</t>
   </si>
 </sst>
 </file>
@@ -340,7 +394,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -636,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223B412C-C145-4BC6-B645-B459A5919E5F}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,9 +701,9 @@
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.7109375" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -816,10 +870,10 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1">
         <v>28941</v>
@@ -836,22 +890,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1249.5999999999999</v>
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>0.20519999999999999</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -859,22 +913,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D10">
-        <v>3054.42</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>24.3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -882,22 +936,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>7137.3</v>
+        <v>3.81</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -905,22 +959,20 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D12">
-        <v>7992</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
+        <v>51.418999999999997</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -928,22 +980,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D13">
-        <v>1216.9000000000001</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
+        <v>9.5920000000000005</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -951,22 +1003,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D14">
-        <v>2081.9</v>
+        <v>377.82400000000001</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -974,22 +1026,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D15">
-        <v>7137.3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
+        <v>13.616</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -997,22 +1046,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D16">
-        <v>7137.3</v>
+        <v>499.39249999999998</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1020,22 +1069,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D17">
-        <v>1610.991</v>
+        <v>10.168100000000001</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1043,50 +1092,68 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>67</v>
       </c>
-      <c r="D18">
-        <v>7137.3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D19">
-        <v>7137.3</v>
+        <v>47.549799999999998</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
       <c r="D20">
-        <v>7137.3</v>
+        <v>142.72999999999999</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1094,45 +1161,45 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D21">
-        <v>4492</v>
+        <v>1428.4</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D22">
-        <v>0.20519999999999999</v>
+        <v>5.133</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1140,19 +1207,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23">
-        <v>24.3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3054.42</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1160,21 +1221,164 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24">
-        <v>3.81</v>
-      </c>
-      <c r="E24" t="s">
-        <v>79</v>
+        <v>84</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1930</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25">
+        <v>7992</v>
+      </c>
+      <c r="F25" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26">
+        <v>1216.9000000000001</v>
+      </c>
+      <c r="F26" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27">
+        <v>2081.9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1930</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29">
+        <v>1930</v>
+      </c>
+      <c r="F29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30">
+        <v>1249.5999999999999</v>
+      </c>
+      <c r="F30" t="s">
+        <v>82</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31">
+        <v>7204.3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32">
+        <v>1610.991</v>
+      </c>
+      <c r="F32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33">
+        <v>4492</v>
+      </c>
+      <c r="F33" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34">
+        <v>17.047499999999999</v>
+      </c>
+      <c r="E34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New script: calcKcatFromActivity; Curated more kcats
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujum\OneDrive\Documentos\GitHub\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C983CD-857F-4B40-BDE1-FA9861EF7A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32D6A80-1073-431B-B5C8-8DFBB9420EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
   <si>
     <t>proteins</t>
   </si>
@@ -333,6 +333,75 @@
   </si>
   <si>
     <t>Limits model with DLKcat priority 3.  Calculated from the specific activity of N. crassa (Brenda)</t>
+  </si>
+  <si>
+    <t>Q6C1X5</t>
+  </si>
+  <si>
+    <t>y000040</t>
+  </si>
+  <si>
+    <t>YALI0F12639g</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3.  Calculated from the specific activity of Aspergillus nidulans (EC 4.2.1.10)</t>
+  </si>
+  <si>
+    <t>Q6CAY2</t>
+  </si>
+  <si>
+    <t>YALI0C23408g</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3.  Calculated from the specific activity of N. crassa (EC 4.2.1.9)</t>
+  </si>
+  <si>
+    <t>Q6CA34</t>
+  </si>
+  <si>
+    <t>y000361</t>
+  </si>
+  <si>
+    <t>YALI0D06281g</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Using kcat of S. cerevisiae (EC 2.4.1.83)</t>
+  </si>
+  <si>
+    <t>y000366</t>
+  </si>
+  <si>
+    <t>Q6C1F3</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Using kcat of S. cerevisiae (EC 4.2.1.11)</t>
+  </si>
+  <si>
+    <t>YALI0F16819g</t>
+  </si>
+  <si>
+    <t>Q6BZU8</t>
+  </si>
+  <si>
+    <t>y000725</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Using kcat of E. coli (EC 3.5.4.9)</t>
+  </si>
+  <si>
+    <t>YALI0F30745g</t>
+  </si>
+  <si>
+    <t>YALI0D20152g</t>
+  </si>
+  <si>
+    <t>Q6C8F2</t>
+  </si>
+  <si>
+    <t>y000760</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Using kcat of Aspergillus fumigatus (EC 2.3.1.4)</t>
   </si>
 </sst>
 </file>
@@ -370,12 +439,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +463,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -690,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223B412C-C145-4BC6-B645-B459A5919E5F}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +898,7 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>28941</v>
       </c>
       <c r="E6" t="s">
@@ -846,13 +915,13 @@
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>28941</v>
       </c>
       <c r="E7" t="s">
@@ -875,7 +944,7 @@
       <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>28941</v>
       </c>
       <c r="E8" t="s">
@@ -970,7 +1039,7 @@
       <c r="D12">
         <v>51.418999999999997</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="2"/>
       <c r="F12" t="s">
         <v>46</v>
       </c>
@@ -991,7 +1060,7 @@
       <c r="D13">
         <v>9.5920000000000005</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F13" t="s">
@@ -1209,7 +1278,7 @@
       <c r="A23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>3054.42</v>
       </c>
       <c r="F23" t="s">
@@ -1223,7 +1292,7 @@
       <c r="A24" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>1930</v>
       </c>
       <c r="F24" t="s">
@@ -1279,7 +1348,7 @@
       <c r="A28" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>1930</v>
       </c>
       <c r="F28" t="s">
@@ -1355,7 +1424,7 @@
       <c r="F33" t="s">
         <v>82</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="3" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1379,6 +1448,141 @@
         <v>98</v>
       </c>
       <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="4">
+        <v>3583.8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36">
+        <v>10.3331</v>
+      </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="E37" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38">
+        <v>230</v>
+      </c>
+      <c r="E38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39">
+        <v>40.9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" t="s">
+        <v>116</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40">
+        <v>38</v>
+      </c>
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" t="s">
+        <v>121</v>
+      </c>
+      <c r="G40">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fine tuning ecYali: f = 0.5 and kcat curation
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujum\OneDrive\Documentos\GitHub\GECKO\ecYaliGEM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32D6A80-1073-431B-B5C8-8DFBB9420EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F386EE-D3BC-4D24-88F6-F820150CD446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
+    <workbookView xWindow="3650" yWindow="14290" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="F 0.3" sheetId="1" r:id="rId1"/>
+    <sheet name="F 0.5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="152">
   <si>
     <t>proteins</t>
   </si>
@@ -224,9 +225,6 @@
     <t>y000354</t>
   </si>
   <si>
-    <t>Output of sensitivityTuning. Calculated from the specific activity of Candida methylica (Brenda) x10.</t>
-  </si>
-  <si>
     <t>y000233</t>
   </si>
   <si>
@@ -245,9 +243,6 @@
     <t>y000219</t>
   </si>
   <si>
-    <t>Limits model with DLKcat priority 5. Calculatedby multiplying highest kcat/Km * Km (Brenda EC 1.14.19.41)</t>
-  </si>
-  <si>
     <t>Limits model with DLKcat priority 5. Calculated from the specific activity of S. cerevisae (Ec 1.2.1.11)</t>
   </si>
   <si>
@@ -402,6 +397,102 @@
   </si>
   <si>
     <t>Limits model with DLKcat priority 3. Using kcat of Aspergillus fumigatus (EC 2.3.1.4)</t>
+  </si>
+  <si>
+    <t>y000910</t>
+  </si>
+  <si>
+    <t>Q6CGV2</t>
+  </si>
+  <si>
+    <t>YALI0A15950g</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Calculated from the specific activity of S. cerevisiae (EC 3.6.1.31)</t>
+  </si>
+  <si>
+    <t>Q6C7Y2</t>
+  </si>
+  <si>
+    <t>y000912</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Using kcat of E. coli (EC 2.1.2.3)</t>
+  </si>
+  <si>
+    <t>YALI0D24409g</t>
+  </si>
+  <si>
+    <t>Q99148</t>
+  </si>
+  <si>
+    <t>YALI0F21010g</t>
+  </si>
+  <si>
+    <t>y000914</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Using kcat of Gallus gallus (EC 6.3.4.13)</t>
+  </si>
+  <si>
+    <t>P38997</t>
+  </si>
+  <si>
+    <t>YALI0B15444g</t>
+  </si>
+  <si>
+    <t>y000988</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 3. Calculated from the specific activity of S. cerevisiae (EC 1.5.1.7)</t>
+  </si>
+  <si>
+    <t>y200001</t>
+  </si>
+  <si>
+    <t>YALI0B23188g</t>
+  </si>
+  <si>
+    <t>Q6CDK7</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 5. Calculatedby multiplying highest kcat/Km * Km (EC 1.14.19.41)</t>
+  </si>
+  <si>
+    <t>Output of sensitivityTuning. Calculated by multiplying highest kcat/Km * Km of Escherichia coli (EC 2.7.1.29).</t>
+  </si>
+  <si>
+    <t>Q6C6H1</t>
+  </si>
+  <si>
+    <t>YALI0E09603g</t>
+  </si>
+  <si>
+    <t>y000470</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2.  Calculated from the specific activity of N. crassa (EC 4.2.1.9)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2.  Calculated from the specific activity of N. crassa (Brenda)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2. Using kcat of S. cerevisiae (EC 4.2.1.11)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2. Calculated from the specific activity of S. cerevisiae (EC 3.6.1.31)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2. Using kcat of E. coli (EC 2.1.2.3)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2. Calculated from the specific activity of S. cerevisiae (EC 1.5.1.7)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2.  Calculated from the specific activity of Aspergillus nidulans (EC 1.4.1.2)</t>
+  </si>
+  <si>
+    <t>Limits model with DLKcat priority 2. Calculated by multiplying highest kcat/Km * Km of Escherichia coli (EC 2.7.1.29)</t>
   </si>
 </sst>
 </file>
@@ -463,7 +554,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -759,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223B412C-C145-4BC6-B645-B459A5919E5F}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,13 +1172,13 @@
         <v>52</v>
       </c>
       <c r="D14">
-        <v>377.82400000000001</v>
+        <v>891</v>
       </c>
       <c r="E14" t="s">
         <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1161,22 +1252,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18">
         <v>0.58399999999999996</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1184,22 +1275,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>47.549799999999998</v>
       </c>
       <c r="E19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" t="s">
         <v>68</v>
-      </c>
-      <c r="F19" t="s">
-        <v>70</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1207,22 +1298,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
         <v>72</v>
       </c>
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D20">
         <v>142.72999999999999</v>
       </c>
       <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
         <v>71</v>
-      </c>
-      <c r="F20" t="s">
-        <v>73</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1230,19 +1321,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D21">
         <v>1428.4</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" t="s">
         <v>46</v>
@@ -1253,22 +1344,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D22">
         <v>5.133</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1276,13 +1367,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" s="2">
         <v>3054.42</v>
       </c>
       <c r="F23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1290,13 +1381,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="2">
         <v>1930</v>
       </c>
       <c r="F24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1304,13 +1395,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D25">
         <v>7992</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1318,13 +1409,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>1216.9000000000001</v>
       </c>
       <c r="F26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1332,13 +1423,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D27">
         <v>2081.9</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1346,13 +1437,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D28" s="2">
         <v>1930</v>
       </c>
       <c r="F28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1360,13 +1451,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D29">
         <v>1930</v>
       </c>
       <c r="F29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1374,13 +1465,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D30">
         <v>1249.5999999999999</v>
       </c>
       <c r="F30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1388,13 +1479,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>7204.3</v>
       </c>
       <c r="F31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1402,13 +1493,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D32">
         <v>1610.991</v>
       </c>
       <c r="F32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1416,36 +1507,36 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D33">
         <v>4492</v>
       </c>
       <c r="F33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D34">
         <v>17.047499999999999</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1453,22 +1544,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
-        <v>101</v>
-      </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D35" s="4">
         <v>3583.8</v>
       </c>
       <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
         <v>100</v>
-      </c>
-      <c r="F35" t="s">
-        <v>102</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -1476,19 +1567,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D36">
         <v>10.3331</v>
       </c>
       <c r="F36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1496,22 +1587,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
         <v>106</v>
       </c>
-      <c r="B37" t="s">
-        <v>108</v>
-      </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D37">
         <v>70.900000000000006</v>
       </c>
       <c r="E37" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" t="s">
         <v>107</v>
-      </c>
-      <c r="F37" t="s">
-        <v>109</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -1519,22 +1610,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
         <v>111</v>
       </c>
-      <c r="B38" t="s">
-        <v>113</v>
-      </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D38">
         <v>230</v>
       </c>
       <c r="E38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" t="s">
         <v>110</v>
-      </c>
-      <c r="F38" t="s">
-        <v>112</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -1542,22 +1633,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D39">
         <v>40.9</v>
       </c>
       <c r="E39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -1565,24 +1656,139 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D40">
         <v>38</v>
       </c>
       <c r="E40" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41">
+        <v>507.79399999999998</v>
+      </c>
+      <c r="E41" t="s">
         <v>120</v>
       </c>
-      <c r="F40" t="s">
-        <v>121</v>
-      </c>
-      <c r="G40">
+      <c r="F41" t="s">
+        <v>123</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42">
+        <v>4.97</v>
+      </c>
+      <c r="E42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" t="s">
+        <v>126</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43">
+        <v>7.2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44">
+        <v>71.747900000000001</v>
+      </c>
+      <c r="E44" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" t="s">
+        <v>135</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45">
+        <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45">
         <v>1</v>
       </c>
     </row>
@@ -1590,4 +1796,298 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFA18-0B26-4075-8698-68669C0E9618}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="98.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2">
+        <v>9.5920000000000005</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3">
+        <v>17.047499999999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>3.81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <v>10.168100000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6">
+        <v>10.3331</v>
+      </c>
+      <c r="F6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7">
+        <v>42.93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8">
+        <v>230</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9">
+        <v>130.53649999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10">
+        <v>507.79399999999998</v>
+      </c>
+      <c r="E10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11">
+        <v>4.97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12">
+        <v>71.747900000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Analysis of newer ecYali
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujum\OneDrive\Documentos\GitHub\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F386EE-D3BC-4D24-88F6-F820150CD446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F64872-6D06-40C2-B17C-945026E9466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3650" yWindow="14290" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
     <sheet name="F 0.3" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="152">
   <si>
     <t>proteins</t>
   </si>
@@ -554,7 +554,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -853,7 +853,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,10 +1800,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFA18-0B26-4075-8698-68669C0E9618}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,6 +2087,164 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>186</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>7.8799999999999995E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>136.96090000000001</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="4">
+        <v>28941</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="4">
+        <v>28941</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="4">
+        <v>28941</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New: better curated proteomics data
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujum\OneDrive\Documentos\GitHub\GECKO\ecYaliGEM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F64872-6D06-40C2-B17C-945026E9466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314A24A1-EB55-4A0D-90A8-6CF711F10ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
     <sheet name="F 0.3" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="154">
   <si>
     <t>proteins</t>
   </si>
@@ -493,6 +493,12 @@
   </si>
   <si>
     <t>Limits model with DLKcat priority 2. Calculated by multiplying highest kcat/Km * Km of Escherichia coli (EC 2.7.1.29)</t>
+  </si>
+  <si>
+    <t>Limits model when adding proteomics data. Calculated from specific activity of E. coli (EC 2.7.8.B10)</t>
+  </si>
+  <si>
+    <t>Limits model when adding proteomics data. Using kcat of Aspergillus fumigatus (EC 2.3.1.4)</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -853,7 +859,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G8"/>
+      <selection activeCell="A40" sqref="A40:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFA18-0B26-4075-8698-68669C0E9618}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,6 +2251,206 @@
         <v>1</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2.6429999999999998</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3054.42</v>
+      </c>
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1930</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23">
+        <v>7992</v>
+      </c>
+      <c r="F23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24">
+        <v>1216.9000000000001</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25">
+        <v>2081.9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1930</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27">
+        <v>1930</v>
+      </c>
+      <c r="F27" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28">
+        <v>1249.5999999999999</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29">
+        <v>7204.3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30">
+        <v>1610.991</v>
+      </c>
+      <c r="F30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31">
+        <v>4492</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Curated more kcats. WT exp ecModel functional
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314A24A1-EB55-4A0D-90A8-6CF711F10ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC01555-5E75-4B6B-ACD2-93816C409559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
     <sheet name="F 0.3" sheetId="1" r:id="rId1"/>
-    <sheet name="F 0.5" sheetId="2" r:id="rId2"/>
+    <sheet name="customKcats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="166">
   <si>
     <t>proteins</t>
   </si>
@@ -499,6 +499,42 @@
   </si>
   <si>
     <t>Limits model when adding proteomics data. Using kcat of Aspergillus fumigatus (EC 2.3.1.4)</t>
+  </si>
+  <si>
+    <t>Q6CAG1</t>
+  </si>
+  <si>
+    <t>Limits model when adding proteomics data. Calculatedby multiplying highest kcat/Km * Km (EC 1.14.19.41)</t>
+  </si>
+  <si>
+    <t>Limits model when adding proteomics data. Calculated from the specific activity of N. crassa (Brenda)</t>
+  </si>
+  <si>
+    <t>YALI0D03069g</t>
+  </si>
+  <si>
+    <t>Q6CE88</t>
+  </si>
+  <si>
+    <t>YALI0B17644g</t>
+  </si>
+  <si>
+    <t>y000236, y000237</t>
+  </si>
+  <si>
+    <t>Limits model when adding proteomics data. Using kcat of E. coli (EC 2.1.2.2)</t>
+  </si>
+  <si>
+    <t>Limits model when adding proteomics data. Using standardKcat.</t>
+  </si>
+  <si>
+    <t>Q6C5R8</t>
+  </si>
+  <si>
+    <t>YALI0E15730g</t>
+  </si>
+  <si>
+    <t>Limits model when adding proteomics data. Using standardKcat/10 instead.</t>
   </si>
 </sst>
 </file>
@@ -859,7 +895,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:G40"/>
+      <selection activeCell="A46" sqref="A46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +905,7 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.7109375" customWidth="1"/>
+    <col min="6" max="6" width="80.140625" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1806,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFA18-0B26-4075-8698-68669C0E9618}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,6 +2487,113 @@
         <v>1</v>
       </c>
     </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" t="s">
+        <v>155</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <v>51.418999999999997</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35">
+        <v>13.5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>161</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36">
+        <v>14.3186</v>
+      </c>
+      <c r="E36" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37">
+        <v>1.4318599999999999</v>
+      </c>
+      <c r="F37" t="s">
+        <v>165</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ecYaliGEM curated for more accurate acetaldehyde metabolism
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC01555-5E75-4B6B-ACD2-93816C409559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F39E69-69EC-4B02-B50A-9971AEAB1B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
     <sheet name="F 0.3" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="176">
   <si>
     <t>proteins</t>
   </si>
@@ -535,6 +535,36 @@
   </si>
   <si>
     <t>Limits model when adding proteomics data. Using standardKcat/10 instead.</t>
+  </si>
+  <si>
+    <t>y000173</t>
+  </si>
+  <si>
+    <t>YALI0C03025g</t>
+  </si>
+  <si>
+    <t>Q6CD79</t>
+  </si>
+  <si>
+    <t>Putative enzyme. Using the lowest kcat instead, which is the one predicted by DLKcat in this case.</t>
+  </si>
+  <si>
+    <t>YALI0D07942g</t>
+  </si>
+  <si>
+    <t>Q6C9V7</t>
+  </si>
+  <si>
+    <t>y000185</t>
+  </si>
+  <si>
+    <t>YALI0F04444g</t>
+  </si>
+  <si>
+    <t>Q6C2W9</t>
+  </si>
+  <si>
+    <t>y002116</t>
   </si>
 </sst>
 </file>
@@ -1842,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFA18-0B26-4075-8698-68669C0E9618}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,6 +2624,121 @@
         <v>1</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38">
+        <v>12.3903</v>
+      </c>
+      <c r="E38" t="s">
+        <v>166</v>
+      </c>
+      <c r="F38" t="s">
+        <v>169</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39">
+        <v>26.515499999999999</v>
+      </c>
+      <c r="E39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F39" t="s">
+        <v>169</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40">
+        <v>32.9861</v>
+      </c>
+      <c r="E40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F40" t="s">
+        <v>169</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41">
+        <v>6.7826000000000004</v>
+      </c>
+      <c r="E41" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" t="s">
+        <v>169</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42">
+        <v>9.1103000000000005</v>
+      </c>
+      <c r="E42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" t="s">
+        <v>169</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New ecYali based on an update of iYali4
</commit_message>
<xml_diff>
--- a/ecYaliGEM/data/customKcats.xlsx
+++ b/ecYaliGEM/data/customKcats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F39E69-69EC-4B02-B50A-9971AEAB1B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7824126F-105E-47AF-8DFA-28A41CF3E450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2C064AA4-60C4-4B2C-B291-699BBD5F96CD}"/>
   </bookViews>
   <sheets>
     <sheet name="F 0.3" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="187">
   <si>
     <t>proteins</t>
   </si>
@@ -565,6 +565,39 @@
   </si>
   <si>
     <t>y002116</t>
+  </si>
+  <si>
+    <t>Q9UVF4</t>
+  </si>
+  <si>
+    <t>YALI0B02948g</t>
+  </si>
+  <si>
+    <t>y000491_REV</t>
+  </si>
+  <si>
+    <t>Limits model after curations of iYali. Calculated from the specific activity of S. cerevisiae (EC 1.1.1.8)</t>
+  </si>
+  <si>
+    <t>Q6C8V3</t>
+  </si>
+  <si>
+    <t>YALI0D16753g</t>
+  </si>
+  <si>
+    <t>y000713</t>
+  </si>
+  <si>
+    <t>Q6C5X9</t>
+  </si>
+  <si>
+    <t>YALI0E14190g</t>
+  </si>
+  <si>
+    <t>kcat from BRENDA was causing overuse of the NADH shuttle. Using value of DLKcat instead.</t>
+  </si>
+  <si>
+    <t>kcat from BRENDA (highest) was causing overuse of the NADH shuttle. Using highest kcat in the same order of magnitude predicted by DLKcat.</t>
   </si>
 </sst>
 </file>
@@ -1872,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFA18-0B26-4075-8698-68669C0E9618}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,6 +2772,75 @@
         <v>1</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>176</v>
+      </c>
+      <c r="B43" t="s">
+        <v>177</v>
+      </c>
+      <c r="C43" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43">
+        <v>114.44199999999999</v>
+      </c>
+      <c r="E43" t="s">
+        <v>178</v>
+      </c>
+      <c r="F43" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" t="s">
+        <v>181</v>
+      </c>
+      <c r="D44">
+        <v>83.2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>182</v>
+      </c>
+      <c r="F44" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" t="s">
+        <v>184</v>
+      </c>
+      <c r="D45">
+        <v>3.1017999999999999</v>
+      </c>
+      <c r="E45" t="s">
+        <v>182</v>
+      </c>
+      <c r="F45" t="s">
+        <v>185</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>